<commit_message>
Add subsets tab bck in
</commit_message>
<xml_diff>
--- a/curation/draft/CDASH_draft.xlsx
+++ b/curation/draft/CDASH_draft.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Linda\Documents\CDISC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\curation\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4254F83-6D2E-474E-9932-67321FEDCF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A5DD9E-AD36-4248-B2A5-7AB69D5ACFB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" firstSheet="1" activeTab="1" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{FA29263D-F7AA-4D0C-AE9B-6B008D3B18BE}"/>
   </bookViews>
   <sheets>
     <sheet name="BC_VS" sheetId="34" r:id="rId1"/>
     <sheet name="CDASH VS" sheetId="25" r:id="rId2"/>
     <sheet name="CDASH LB BC" sheetId="11" r:id="rId3"/>
     <sheet name="CDASH DS BC" sheetId="16" r:id="rId4"/>
+    <sheet name="Subset Codelist Example" sheetId="35" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'CDASH LB BC'!$A$1:$AE$1</definedName>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3665" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4177" uniqueCount="749">
   <si>
     <t>C164634</t>
   </si>
@@ -1647,12 +1648,693 @@
   <si>
     <t>SpO2; OXYSAT; O2 Saturation; Hemoglobin Saturation; Oximetry</t>
   </si>
+  <si>
+    <t>Subset Short Name</t>
+  </si>
+  <si>
+    <t>Subset Label</t>
+  </si>
+  <si>
+    <t>Parent Codelist</t>
+  </si>
+  <si>
+    <t>Submission Value</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>NY_Y</t>
+  </si>
+  <si>
+    <t>Yes Response Only</t>
+  </si>
+  <si>
+    <t>C49488</t>
+  </si>
+  <si>
+    <t>NY_NY</t>
+  </si>
+  <si>
+    <t>No Yes Response Only</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>C49487</t>
+  </si>
+  <si>
+    <t>VSRESU_HT</t>
+  </si>
+  <si>
+    <t>Vital Sign Height Unit</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>C48500</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>C49668</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>C41139</t>
+  </si>
+  <si>
+    <t>VSRESU_WT</t>
+  </si>
+  <si>
+    <t>Vital Sign Weight Unit</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>C28252</t>
+  </si>
+  <si>
+    <t>C48531</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>C48155</t>
+  </si>
+  <si>
+    <t>UNIT_BMI</t>
+  </si>
+  <si>
+    <t>Vital Sign BMI Unit</t>
+  </si>
+  <si>
+    <t>kg/m2</t>
+  </si>
+  <si>
+    <t>C49671</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>C67334</t>
+  </si>
+  <si>
+    <t>VSRESU_TEMP</t>
+  </si>
+  <si>
+    <t>Vital Sign Temperature Unit</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C42559</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>C44277</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>C42537</t>
+  </si>
+  <si>
+    <t>VSRESU_WSTCIR</t>
+  </si>
+  <si>
+    <t>Vital Sign Waist Circumference Unit</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>C28251</t>
+  </si>
+  <si>
+    <t>Vital Signs Position</t>
+  </si>
+  <si>
+    <t>SITTING</t>
+  </si>
+  <si>
+    <t>C62122</t>
+  </si>
+  <si>
+    <t>STANDING</t>
+  </si>
+  <si>
+    <t>C62166</t>
+  </si>
+  <si>
+    <t>SUPINE</t>
+  </si>
+  <si>
+    <t>C62167</t>
+  </si>
+  <si>
+    <t>VSLOC_BP</t>
+  </si>
+  <si>
+    <t>Vital Signs BP Anatomic Location</t>
+  </si>
+  <si>
+    <t>ARM</t>
+  </si>
+  <si>
+    <t>C32141</t>
+  </si>
+  <si>
+    <t>FOREARM</t>
+  </si>
+  <si>
+    <t>C32628</t>
+  </si>
+  <si>
+    <t>THIGH</t>
+  </si>
+  <si>
+    <t>C33763</t>
+  </si>
+  <si>
+    <t>CALF</t>
+  </si>
+  <si>
+    <t>C93027</t>
+  </si>
+  <si>
+    <t>ARTERY</t>
+  </si>
+  <si>
+    <t>C12372</t>
+  </si>
+  <si>
+    <t>VSLAT_BP</t>
+  </si>
+  <si>
+    <t>Vital Signs BP Laterality</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>C25228</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>C25229</t>
+  </si>
+  <si>
+    <t>VSLOC_PULSE</t>
+  </si>
+  <si>
+    <t>Vital Signs Pulse Rate Location</t>
+  </si>
+  <si>
+    <t>BRACHIAL ARTERY</t>
+  </si>
+  <si>
+    <t>C12681</t>
+  </si>
+  <si>
+    <t>COROTID ARTERY</t>
+  </si>
+  <si>
+    <t>C12687</t>
+  </si>
+  <si>
+    <t>DORSALIS PEDIS ARTERY</t>
+  </si>
+  <si>
+    <t>C32478</t>
+  </si>
+  <si>
+    <t>FEMORAL ARTERY</t>
+  </si>
+  <si>
+    <t>C12715</t>
+  </si>
+  <si>
+    <t>RADIAL ARTERY</t>
+  </si>
+  <si>
+    <t>C12838</t>
+  </si>
+  <si>
+    <t>VSLOC_TEMP</t>
+  </si>
+  <si>
+    <t>Vital Signs Body Temperature Location</t>
+  </si>
+  <si>
+    <t>AXILLA</t>
+  </si>
+  <si>
+    <t>C12674</t>
+  </si>
+  <si>
+    <t>EAR</t>
+  </si>
+  <si>
+    <t>C12394</t>
+  </si>
+  <si>
+    <t>FOREHEAD</t>
+  </si>
+  <si>
+    <t>C89803</t>
+  </si>
+  <si>
+    <t>ORAL CAVITY</t>
+  </si>
+  <si>
+    <t>C12421</t>
+  </si>
+  <si>
+    <t>RECTUM</t>
+  </si>
+  <si>
+    <t>C12390</t>
+  </si>
+  <si>
+    <t>UNIT_MCNC</t>
+  </si>
+  <si>
+    <t>Unit of Mass Concentration</t>
+  </si>
+  <si>
+    <t>g/dL</t>
+  </si>
+  <si>
+    <t>C64783</t>
+  </si>
+  <si>
+    <t>g/L</t>
+  </si>
+  <si>
+    <t>C42576</t>
+  </si>
+  <si>
+    <t>kg/L</t>
+  </si>
+  <si>
+    <t>C64566</t>
+  </si>
+  <si>
+    <t>mg/dL</t>
+  </si>
+  <si>
+    <t>C67015</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>C64572</t>
+  </si>
+  <si>
+    <t>ng/dL</t>
+  </si>
+  <si>
+    <t>C67326</t>
+  </si>
+  <si>
+    <t>ng/L</t>
+  </si>
+  <si>
+    <t>C67327</t>
+  </si>
+  <si>
+    <t>pg/dL</t>
+  </si>
+  <si>
+    <t>C67331</t>
+  </si>
+  <si>
+    <t>pg/L</t>
+  </si>
+  <si>
+    <t>C85597</t>
+  </si>
+  <si>
+    <t>ug/dL</t>
+  </si>
+  <si>
+    <t>C67305</t>
+  </si>
+  <si>
+    <t>DTM</t>
+  </si>
+  <si>
+    <t>ug/L</t>
+  </si>
+  <si>
+    <t>C67306</t>
+  </si>
+  <si>
+    <t>UNIT_SCNC</t>
+  </si>
+  <si>
+    <t>Unit of Substance Concentration</t>
+  </si>
+  <si>
+    <t>mEq/L</t>
+  </si>
+  <si>
+    <t>C67474</t>
+  </si>
+  <si>
+    <t>mmol/L</t>
+  </si>
+  <si>
+    <t>C64387</t>
+  </si>
+  <si>
+    <t>umol/L</t>
+  </si>
+  <si>
+    <t>C48508</t>
+  </si>
+  <si>
+    <t>cmol/L</t>
+  </si>
+  <si>
+    <t>C68886</t>
+  </si>
+  <si>
+    <t>damol/L</t>
+  </si>
+  <si>
+    <t>C105483</t>
+  </si>
+  <si>
+    <t>fmol/L</t>
+  </si>
+  <si>
+    <t>C68887</t>
+  </si>
+  <si>
+    <t>mEq/dL</t>
+  </si>
+  <si>
+    <t>C67473</t>
+  </si>
+  <si>
+    <t>mEq/mL</t>
+  </si>
+  <si>
+    <t>C73737</t>
+  </si>
+  <si>
+    <t>mEq/uL</t>
+  </si>
+  <si>
+    <t>C70578</t>
+  </si>
+  <si>
+    <t>mol/L</t>
+  </si>
+  <si>
+    <t>C48555</t>
+  </si>
+  <si>
+    <t>mol/mL</t>
+  </si>
+  <si>
+    <t>C68891</t>
+  </si>
+  <si>
+    <t>nmol/L</t>
+  </si>
+  <si>
+    <t>C67432</t>
+  </si>
+  <si>
+    <t>pmol/L</t>
+  </si>
+  <si>
+    <t>C67434</t>
+  </si>
+  <si>
+    <t>uEq/L</t>
+  </si>
+  <si>
+    <t>C117975</t>
+  </si>
+  <si>
+    <t>UNIT_MASS</t>
+  </si>
+  <si>
+    <t>Unit of Mass</t>
+  </si>
+  <si>
+    <t>ag</t>
+  </si>
+  <si>
+    <t>C64553</t>
+  </si>
+  <si>
+    <t>amu</t>
+  </si>
+  <si>
+    <t>C64559</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>C64554</t>
+  </si>
+  <si>
+    <t>dram</t>
+  </si>
+  <si>
+    <t>C64564</t>
+  </si>
+  <si>
+    <t>fg</t>
+  </si>
+  <si>
+    <t>C64552</t>
+  </si>
+  <si>
+    <t>grain</t>
+  </si>
+  <si>
+    <t>C48497</t>
+  </si>
+  <si>
+    <t>kDa</t>
+  </si>
+  <si>
+    <t>C105491</t>
+  </si>
+  <si>
+    <t>mg</t>
+  </si>
+  <si>
+    <t>C28253</t>
+  </si>
+  <si>
+    <t>ng</t>
+  </si>
+  <si>
+    <t>C48516</t>
+  </si>
+  <si>
+    <t>oz</t>
+  </si>
+  <si>
+    <t>C48519</t>
+  </si>
+  <si>
+    <t>pg</t>
+  </si>
+  <si>
+    <t>C64551</t>
+  </si>
+  <si>
+    <t>ug</t>
+  </si>
+  <si>
+    <t>C48152</t>
+  </si>
+  <si>
+    <t>UNIT_CCNC</t>
+  </si>
+  <si>
+    <t>Unit of Catalytic Concentration</t>
+  </si>
+  <si>
+    <t>mU/L</t>
+  </si>
+  <si>
+    <t>C67408</t>
+  </si>
+  <si>
+    <t>nU/cL</t>
+  </si>
+  <si>
+    <t>C105513</t>
+  </si>
+  <si>
+    <t>U/cL</t>
+  </si>
+  <si>
+    <t>C105520</t>
+  </si>
+  <si>
+    <t>U/dL</t>
+  </si>
+  <si>
+    <t>C105521</t>
+  </si>
+  <si>
+    <t>U/L</t>
+  </si>
+  <si>
+    <t>C67456</t>
+  </si>
+  <si>
+    <t>U/mL</t>
+  </si>
+  <si>
+    <t>C77607</t>
+  </si>
+  <si>
+    <t>nkat/L</t>
+  </si>
+  <si>
+    <t>C70510</t>
+  </si>
+  <si>
+    <t>ukat/L</t>
+  </si>
+  <si>
+    <t>C67397</t>
+  </si>
+  <si>
+    <t>UNIT_NCNC</t>
+  </si>
+  <si>
+    <t>Unit of Number Concentration</t>
+  </si>
+  <si>
+    <t>10^9/L</t>
+  </si>
+  <si>
+    <t>C67255</t>
+  </si>
+  <si>
+    <t>/uL</t>
+  </si>
+  <si>
+    <t>C67254</t>
+  </si>
+  <si>
+    <t>CVFARS_MITYPE</t>
+  </si>
+  <si>
+    <t>Acute Myocardial Infarction Type</t>
+  </si>
+  <si>
+    <t>C119016</t>
+  </si>
+  <si>
+    <t>TYPE 1 MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119220</t>
+  </si>
+  <si>
+    <t>TYPE 2 MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119221</t>
+  </si>
+  <si>
+    <t>TYPE 3 MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119222</t>
+  </si>
+  <si>
+    <t>TYPE 4A MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119223</t>
+  </si>
+  <si>
+    <t>TYPE 4B MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119224</t>
+  </si>
+  <si>
+    <t>TYPE 4C MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119225</t>
+  </si>
+  <si>
+    <t>TYPE 5 MYOCARDIAL INFARCTION</t>
+  </si>
+  <si>
+    <t>C119226</t>
+  </si>
+  <si>
+    <t>EVAL_EG</t>
+  </si>
+  <si>
+    <t>Electrocardiogram Evaluator</t>
+  </si>
+  <si>
+    <t>C78735</t>
+  </si>
+  <si>
+    <t>ADJUDICATION COMMITTEE</t>
+  </si>
+  <si>
+    <t>C78726</t>
+  </si>
+  <si>
+    <t>INVESTIGATOR</t>
+  </si>
+  <si>
+    <t>C25936</t>
+  </si>
+  <si>
+    <t>VENDOR</t>
+  </si>
+  <si>
+    <t>C68608</t>
+  </si>
+  <si>
+    <t>INDEPENDENT ASSESSOR</t>
+  </si>
+  <si>
+    <t>C78720</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1731,6 +2413,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1758,7 +2445,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1781,12 +2468,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="1" tint="0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1867,6 +2580,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2188,24 +2911,24 @@
       <selection activeCell="N6" sqref="L6:N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5859375" customWidth="1"/>
-    <col min="2" max="2" width="18.17578125" customWidth="1"/>
-    <col min="3" max="3" width="6.8203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.3515625" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.64453125" customWidth="1"/>
-    <col min="7" max="7" width="11.234375" customWidth="1"/>
-    <col min="8" max="8" width="52.234375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.703125" customWidth="1"/>
-    <col min="10" max="10" width="7.234375" customWidth="1"/>
-    <col min="11" max="11" width="6.46875" customWidth="1"/>
-    <col min="13" max="13" width="19.9375" customWidth="1"/>
-    <col min="15" max="15" width="12.64453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="7.28515625" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="15" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:17" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>227</v>
       </c>
@@ -2255,7 +2978,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:17" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>505</v>
       </c>
@@ -2286,7 +3009,7 @@
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
     </row>
-    <row r="3" spans="1:17" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>505</v>
       </c>
@@ -2323,7 +3046,7 @@
       <c r="L3" s="39"/>
       <c r="Q3" s="40"/>
     </row>
-    <row r="4" spans="1:17" ht="15.45" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:17" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>505</v>
       </c>
@@ -2353,7 +3076,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>505</v>
       </c>
@@ -2386,7 +3109,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>505</v>
       </c>
@@ -2440,42 +3163,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46625CF1-27D2-4F83-88B5-2D336D68510E}">
   <dimension ref="A1:AE80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.17578125" customWidth="1"/>
-    <col min="5" max="5" width="5.87890625" customWidth="1"/>
-    <col min="6" max="6" width="6.703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.64453125" customWidth="1"/>
-    <col min="8" max="8" width="19.8203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.76171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.76171875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.76171875" customWidth="1"/>
-    <col min="12" max="12" width="60.41015625" customWidth="1"/>
-    <col min="13" max="13" width="25.9375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.52734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.64453125" customWidth="1"/>
-    <col min="19" max="19" width="33.17578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.64453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.17578125" customWidth="1"/>
-    <col min="22" max="22" width="13.52734375" customWidth="1"/>
-    <col min="24" max="24" width="23.46875" customWidth="1"/>
-    <col min="25" max="25" width="21.76171875" customWidth="1"/>
-    <col min="26" max="26" width="15.3515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.76171875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.87890625" customWidth="1"/>
-    <col min="29" max="29" width="15.5859375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.5859375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.3515625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="12" max="12" width="60.42578125" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" customWidth="1"/>
+    <col min="19" max="19" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" customWidth="1"/>
+    <col min="25" max="25" width="21.7109375" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.85546875" customWidth="1"/>
+    <col min="29" max="29" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:31" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>227</v>
       </c>
@@ -2570,7 +3293,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>472</v>
       </c>
@@ -2638,7 +3361,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>472</v>
       </c>
@@ -2721,7 +3444,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>472</v>
       </c>
@@ -2789,7 +3512,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>472</v>
       </c>
@@ -2872,7 +3595,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>472</v>
       </c>
@@ -2940,7 +3663,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>472</v>
       </c>
@@ -3017,7 +3740,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="1:31" ht="43" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:31" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>472</v>
       </c>
@@ -3094,7 +3817,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="43" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>472</v>
       </c>
@@ -3171,7 +3894,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="10" spans="1:31" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>472</v>
       </c>
@@ -3248,7 +3971,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>472</v>
       </c>
@@ -3316,7 +4039,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>472</v>
       </c>
@@ -3393,7 +4116,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="13" spans="1:31" ht="43" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:31" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>472</v>
       </c>
@@ -3470,7 +4193,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:31" ht="43" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:31" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>472</v>
       </c>
@@ -3547,7 +4270,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="15" spans="1:31" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>472</v>
       </c>
@@ -3624,7 +4347,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>472</v>
       </c>
@@ -3692,7 +4415,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>472</v>
       </c>
@@ -3769,7 +4492,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="18" spans="1:30" ht="43" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>472</v>
       </c>
@@ -3846,7 +4569,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="19" spans="1:30" ht="43" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:30" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>472</v>
       </c>
@@ -3923,7 +4646,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="20" spans="1:30" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>472</v>
       </c>
@@ -4000,7 +4723,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>472</v>
       </c>
@@ -4068,7 +4791,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>472</v>
       </c>
@@ -4148,7 +4871,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>472</v>
       </c>
@@ -4225,7 +4948,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>472</v>
       </c>
@@ -4293,7 +5016,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>472</v>
       </c>
@@ -4370,7 +5093,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="26" spans="1:30" ht="43" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>472</v>
       </c>
@@ -4447,7 +5170,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="27" spans="1:30" ht="43" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:30" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>472</v>
       </c>
@@ -4524,7 +5247,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>472</v>
       </c>
@@ -4601,7 +5324,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>472</v>
       </c>
@@ -4669,7 +5392,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>472</v>
       </c>
@@ -4749,7 +5472,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="31" spans="1:30" ht="43" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:30" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>472</v>
       </c>
@@ -4826,7 +5549,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>472</v>
       </c>
@@ -4894,7 +5617,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>472</v>
       </c>
@@ -4974,7 +5697,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>472</v>
       </c>
@@ -5039,7 +5762,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:30" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>472</v>
       </c>
@@ -5116,7 +5839,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="36" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="22" t="s">
         <v>472</v>
       </c>
@@ -5180,7 +5903,7 @@
       <c r="AC36" s="29"/>
       <c r="AD36" s="14"/>
     </row>
-    <row r="37" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="22" t="s">
         <v>472</v>
       </c>
@@ -5248,7 +5971,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="38" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
         <v>472</v>
       </c>
@@ -5331,7 +6054,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="39" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
         <v>472</v>
       </c>
@@ -5395,7 +6118,7 @@
       <c r="AC39" s="29"/>
       <c r="AD39" s="14"/>
     </row>
-    <row r="40" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
         <v>472</v>
       </c>
@@ -5463,7 +6186,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="41" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
         <v>472</v>
       </c>
@@ -5546,7 +6269,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="42" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
         <v>472</v>
       </c>
@@ -5610,7 +6333,7 @@
       <c r="AC42" s="29"/>
       <c r="AD42" s="14"/>
     </row>
-    <row r="43" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
         <v>472</v>
       </c>
@@ -5678,7 +6401,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="44" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
         <v>472</v>
       </c>
@@ -5755,7 +6478,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="45" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:30" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
         <v>472</v>
       </c>
@@ -5832,7 +6555,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="46" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:30" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
         <v>472</v>
       </c>
@@ -5909,7 +6632,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="47" spans="1:30" s="23" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>472</v>
       </c>
@@ -5986,7 +6709,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="48" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
         <v>472</v>
       </c>
@@ -6050,7 +6773,7 @@
       <c r="AC48" s="29"/>
       <c r="AD48" s="14"/>
     </row>
-    <row r="49" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="22" t="s">
         <v>472</v>
       </c>
@@ -6118,7 +6841,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="50" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>472</v>
       </c>
@@ -6195,7 +6918,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="51" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:30" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="22" t="s">
         <v>472</v>
       </c>
@@ -6272,7 +6995,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="52" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:30" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
         <v>472</v>
       </c>
@@ -6349,7 +7072,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="53" spans="1:30" s="23" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="22" t="s">
         <v>472</v>
       </c>
@@ -6426,7 +7149,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="54" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="22" t="s">
         <v>472</v>
       </c>
@@ -6490,7 +7213,7 @@
       <c r="AC54" s="29"/>
       <c r="AD54" s="14"/>
     </row>
-    <row r="55" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>472</v>
       </c>
@@ -6558,7 +7281,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="56" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>472</v>
       </c>
@@ -6635,7 +7358,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="57" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:30" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="22" t="s">
         <v>472</v>
       </c>
@@ -6712,7 +7435,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="58" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:30" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="22" t="s">
         <v>472</v>
       </c>
@@ -6789,7 +7512,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="59" spans="1:30" s="23" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="22" t="s">
         <v>472</v>
       </c>
@@ -6866,7 +7589,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="60" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="22" t="s">
         <v>472</v>
       </c>
@@ -6930,7 +7653,7 @@
       <c r="AC60" s="29"/>
       <c r="AD60" s="14"/>
     </row>
-    <row r="61" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="22" t="s">
         <v>472</v>
       </c>
@@ -6998,7 +7721,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="62" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="22" t="s">
         <v>472</v>
       </c>
@@ -7078,7 +7801,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="63" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="22" t="s">
         <v>472</v>
       </c>
@@ -7142,7 +7865,7 @@
       <c r="AC63" s="29"/>
       <c r="AD63" s="14"/>
     </row>
-    <row r="64" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
         <v>472</v>
       </c>
@@ -7219,7 +7942,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="65" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="22" t="s">
         <v>472</v>
       </c>
@@ -7283,7 +8006,7 @@
       <c r="AC65" s="29"/>
       <c r="AD65" s="14"/>
     </row>
-    <row r="66" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="22" t="s">
         <v>472</v>
       </c>
@@ -7351,7 +8074,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="67" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="22" t="s">
         <v>472</v>
       </c>
@@ -7428,7 +8151,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="68" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:30" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="22" t="s">
         <v>472</v>
       </c>
@@ -7505,7 +8228,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="69" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:30" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A69" s="22" t="s">
         <v>472</v>
       </c>
@@ -7582,7 +8305,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="70" spans="1:30" s="23" customFormat="1" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="22" t="s">
         <v>472</v>
       </c>
@@ -7659,7 +8382,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="71" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="22" t="s">
         <v>472</v>
       </c>
@@ -7723,7 +8446,7 @@
       <c r="AC71" s="29"/>
       <c r="AD71" s="14"/>
     </row>
-    <row r="72" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="22" t="s">
         <v>472</v>
       </c>
@@ -7791,7 +8514,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="73" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="22" t="s">
         <v>472</v>
       </c>
@@ -7871,7 +8594,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="74" spans="1:30" s="23" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:30" s="23" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A74" s="22" t="s">
         <v>472</v>
       </c>
@@ -7948,7 +8671,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="75" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="22" t="s">
         <v>472</v>
       </c>
@@ -8012,7 +8735,7 @@
       <c r="AC75" s="29"/>
       <c r="AD75" s="14"/>
     </row>
-    <row r="76" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="22" t="s">
         <v>472</v>
       </c>
@@ -8080,7 +8803,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="77" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="22" t="s">
         <v>472</v>
       </c>
@@ -8160,7 +8883,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="78" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="22" t="s">
         <v>472</v>
       </c>
@@ -8224,7 +8947,7 @@
       <c r="AC78" s="29"/>
       <c r="AD78" s="14"/>
     </row>
-    <row r="79" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="22" t="s">
         <v>472</v>
       </c>
@@ -8289,7 +9012,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="80" spans="1:30" s="23" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:30" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="22" t="s">
         <v>472</v>
       </c>
@@ -8454,42 +9177,42 @@
       <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.41015625" customWidth="1"/>
-    <col min="2" max="2" width="7.8203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.8203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="5.5859375" customWidth="1"/>
-    <col min="5" max="5" width="5.05859375" customWidth="1"/>
-    <col min="6" max="6" width="6.17578125" customWidth="1"/>
-    <col min="7" max="7" width="15.41015625" customWidth="1"/>
-    <col min="8" max="8" width="47.1171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.46875" customWidth="1"/>
-    <col min="10" max="10" width="16.87890625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.52734375" customWidth="1"/>
-    <col min="12" max="12" width="36.76171875" customWidth="1"/>
-    <col min="13" max="13" width="16.703125" customWidth="1"/>
-    <col min="14" max="14" width="10.1171875" customWidth="1"/>
-    <col min="15" max="15" width="8.1171875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.52734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1171875" customWidth="1"/>
-    <col min="18" max="18" width="11.76171875" customWidth="1"/>
-    <col min="19" max="19" width="33.1171875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.3515625" customWidth="1"/>
-    <col min="21" max="21" width="9.234375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.29296875" customWidth="1"/>
-    <col min="23" max="23" width="15.52734375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.17578125" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="5" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.140625" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" customWidth="1"/>
+    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.28515625" customWidth="1"/>
+    <col min="23" max="23" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" customWidth="1"/>
     <col min="25" max="25" width="15" customWidth="1"/>
-    <col min="26" max="26" width="27.703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="24.5859375" customWidth="1"/>
-    <col min="29" max="29" width="22.05859375" customWidth="1"/>
+    <col min="26" max="26" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="24.5703125" customWidth="1"/>
+    <col min="29" max="29" width="22" customWidth="1"/>
     <col min="30" max="30" width="8" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.1171875" customWidth="1"/>
+    <col min="31" max="31" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>227</v>
       </c>
@@ -8587,7 +9310,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>472</v>
       </c>
@@ -8656,7 +9379,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>472</v>
       </c>
@@ -8733,7 +9456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>472</v>
       </c>
@@ -8791,7 +9514,7 @@
       </c>
       <c r="AA4" s="8"/>
     </row>
-    <row r="5" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>472</v>
       </c>
@@ -8865,7 +9588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>472</v>
       </c>
@@ -8932,7 +9655,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>472</v>
       </c>
@@ -9012,7 +9735,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>472</v>
       </c>
@@ -9079,7 +9802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>472</v>
       </c>
@@ -9156,7 +9879,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>472</v>
       </c>
@@ -9212,7 +9935,7 @@
       </c>
       <c r="AA10" s="8"/>
     </row>
-    <row r="11" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>472</v>
       </c>
@@ -9286,7 +10009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>472</v>
       </c>
@@ -9354,7 +10077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>472</v>
       </c>
@@ -9434,7 +10157,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>472</v>
       </c>
@@ -9501,7 +10224,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:32" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>472</v>
       </c>
@@ -9578,7 +10301,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:32" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>472</v>
       </c>
@@ -9634,7 +10357,7 @@
       </c>
       <c r="AA16" s="8"/>
     </row>
-    <row r="17" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>472</v>
       </c>
@@ -9708,7 +10431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>472</v>
       </c>
@@ -9776,7 +10499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>472</v>
       </c>
@@ -9856,7 +10579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>472</v>
       </c>
@@ -9923,7 +10646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>472</v>
       </c>
@@ -10000,7 +10723,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>472</v>
       </c>
@@ -10056,7 +10779,7 @@
       </c>
       <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>472</v>
       </c>
@@ -10130,7 +10853,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>472</v>
       </c>
@@ -10196,7 +10919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>472</v>
       </c>
@@ -10274,7 +10997,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>472</v>
       </c>
@@ -10341,7 +11064,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>472</v>
       </c>
@@ -10418,7 +11141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>472</v>
       </c>
@@ -10474,7 +11197,7 @@
       </c>
       <c r="AA28" s="8"/>
     </row>
-    <row r="29" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>472</v>
       </c>
@@ -10548,7 +11271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>472</v>
       </c>
@@ -10614,7 +11337,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>472</v>
       </c>
@@ -10692,7 +11415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>472</v>
       </c>
@@ -10759,7 +11482,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>472</v>
       </c>
@@ -10836,7 +11559,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>472</v>
       </c>
@@ -10892,7 +11615,7 @@
       </c>
       <c r="AA34" s="8"/>
     </row>
-    <row r="35" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>472</v>
       </c>
@@ -10966,7 +11689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>472</v>
       </c>
@@ -11032,7 +11755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>472</v>
       </c>
@@ -11110,7 +11833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>472</v>
       </c>
@@ -11177,7 +11900,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>472</v>
       </c>
@@ -11254,7 +11977,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>472</v>
       </c>
@@ -11310,7 +12033,7 @@
       </c>
       <c r="AA40" s="8"/>
     </row>
-    <row r="41" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>472</v>
       </c>
@@ -11384,7 +12107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>472</v>
       </c>
@@ -11450,7 +12173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>472</v>
       </c>
@@ -11528,7 +12251,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>472</v>
       </c>
@@ -11595,7 +12318,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>472</v>
       </c>
@@ -11672,7 +12395,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>472</v>
       </c>
@@ -11728,7 +12451,7 @@
       </c>
       <c r="AA46" s="8"/>
     </row>
-    <row r="47" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>472</v>
       </c>
@@ -11802,7 +12525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>472</v>
       </c>
@@ -11868,7 +12591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>472</v>
       </c>
@@ -11946,7 +12669,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>472</v>
       </c>
@@ -12013,7 +12736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>472</v>
       </c>
@@ -12090,7 +12813,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>472</v>
       </c>
@@ -12146,7 +12869,7 @@
       </c>
       <c r="AA52" s="8"/>
     </row>
-    <row r="53" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>472</v>
       </c>
@@ -12220,7 +12943,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>472</v>
       </c>
@@ -12286,7 +13009,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>472</v>
       </c>
@@ -12361,7 +13084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>472</v>
       </c>
@@ -12428,7 +13151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="57" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>472</v>
       </c>
@@ -12505,7 +13228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>472</v>
       </c>
@@ -12561,7 +13284,7 @@
       </c>
       <c r="AA58" s="8"/>
     </row>
-    <row r="59" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="59" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>472</v>
       </c>
@@ -12635,7 +13358,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="60" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>472</v>
       </c>
@@ -12701,7 +13424,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="61" spans="1:30" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>472</v>
       </c>
@@ -12779,7 +13502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="62" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D62" s="11"/>
       <c r="E62" s="8"/>
       <c r="F62" s="8"/>
@@ -12791,7 +13514,7 @@
       <c r="W62" s="8"/>
       <c r="X62" s="8"/>
     </row>
-    <row r="63" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="63" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D63" s="11"/>
       <c r="E63" s="8"/>
       <c r="F63" s="8"/>
@@ -12803,7 +13526,7 @@
       <c r="W63" s="8"/>
       <c r="X63" s="8"/>
     </row>
-    <row r="64" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="64" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D64" s="11"/>
       <c r="E64" s="8"/>
       <c r="F64" s="8"/>
@@ -12815,7 +13538,7 @@
       <c r="W64" s="8"/>
       <c r="X64" s="8"/>
     </row>
-    <row r="65" spans="4:24" s="4" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="65" spans="4:24" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D65" s="11"/>
       <c r="E65" s="8"/>
       <c r="F65" s="8"/>
@@ -12827,75 +13550,75 @@
       <c r="W65" s="8"/>
       <c r="X65" s="8"/>
     </row>
-    <row r="66" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="66" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
     </row>
-    <row r="68" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="68" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
     </row>
-    <row r="70" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="70" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
     </row>
-    <row r="72" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="72" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
     </row>
-    <row r="74" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="74" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
     </row>
-    <row r="76" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="76" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
     </row>
-    <row r="78" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="78" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
     </row>
-    <row r="80" spans="4:24" x14ac:dyDescent="0.5">
+    <row r="80" spans="4:24" x14ac:dyDescent="0.25">
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.5">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
     </row>
@@ -12949,36 +13672,36 @@
       <selection pane="bottomLeft" activeCell="AC37" sqref="AC37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="5.05859375" customWidth="1"/>
-    <col min="5" max="5" width="6.05859375" customWidth="1"/>
-    <col min="6" max="6" width="11.05859375" customWidth="1"/>
-    <col min="7" max="7" width="23.46875" customWidth="1"/>
-    <col min="8" max="8" width="5.46875" customWidth="1"/>
-    <col min="9" max="9" width="12.9375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.5859375" customWidth="1"/>
-    <col min="11" max="11" width="36.87890625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.17578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.234375" customWidth="1"/>
-    <col min="16" max="16" width="8.5859375" customWidth="1"/>
-    <col min="17" max="17" width="10.703125" customWidth="1"/>
-    <col min="18" max="18" width="38.17578125" customWidth="1"/>
-    <col min="19" max="19" width="12.05859375" customWidth="1"/>
-    <col min="20" max="20" width="10.5859375" customWidth="1"/>
-    <col min="21" max="21" width="13.5859375" customWidth="1"/>
-    <col min="22" max="22" width="11.234375" customWidth="1"/>
-    <col min="23" max="23" width="14.17578125" customWidth="1"/>
-    <col min="24" max="24" width="10.703125" customWidth="1"/>
-    <col min="25" max="25" width="37.05859375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.17578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.5859375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.8203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5703125" customWidth="1"/>
+    <col min="11" max="11" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="38.140625" customWidth="1"/>
+    <col min="19" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" customWidth="1"/>
+    <col min="23" max="23" width="14.140625" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" customWidth="1"/>
+    <col min="25" max="25" width="37" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:30" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>227</v>
       </c>
@@ -13070,7 +13793,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="4" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:30" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>472</v>
       </c>
@@ -13128,7 +13851,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>472</v>
       </c>
@@ -13189,7 +13912,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>472</v>
       </c>
@@ -13235,7 +13958,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>472</v>
       </c>
@@ -13297,7 +14020,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="4" customFormat="1" ht="71.7" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:30" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>472</v>
       </c>
@@ -13358,7 +14081,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>472</v>
       </c>
@@ -13420,7 +14143,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>472</v>
       </c>
@@ -13467,7 +14190,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>472</v>
       </c>
@@ -13528,7 +14251,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="4" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:30" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>472</v>
       </c>
@@ -13589,7 +14312,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>472</v>
       </c>
@@ -13651,7 +14374,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>472</v>
       </c>
@@ -13698,7 +14421,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>472</v>
       </c>
@@ -13759,7 +14482,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="14" spans="1:30" s="4" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:30" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>472</v>
       </c>
@@ -13820,7 +14543,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>472</v>
       </c>
@@ -13882,7 +14605,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>472</v>
       </c>
@@ -13929,7 +14652,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>472</v>
       </c>
@@ -13990,7 +14713,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="4" customFormat="1" ht="15.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:29" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>472</v>
       </c>
@@ -14051,7 +14774,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:29" ht="15.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>472</v>
       </c>
@@ -14110,7 +14833,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="15.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>472</v>
       </c>
@@ -14157,7 +14880,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="21" spans="1:29" ht="15.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>472</v>
       </c>
@@ -14215,7 +14938,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="22" spans="1:29" ht="15.7" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>472</v>
       </c>
@@ -14277,7 +15000,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>472</v>
       </c>
@@ -14338,7 +15061,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>472</v>
       </c>
@@ -14385,7 +15108,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>472</v>
       </c>
@@ -14446,7 +15169,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>472</v>
       </c>
@@ -14508,7 +15231,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>472</v>
       </c>
@@ -14569,7 +15292,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>472</v>
       </c>
@@ -14616,7 +15339,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>472</v>
       </c>
@@ -14677,7 +15400,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>472</v>
       </c>
@@ -14739,7 +15462,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>472</v>
       </c>
@@ -14800,7 +15523,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>472</v>
       </c>
@@ -14847,7 +15570,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>472</v>
       </c>
@@ -14908,82 +15631,82 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J35" s="4"/>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J37" s="4"/>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J39" s="4"/>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J41" s="4"/>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J43" s="4"/>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J45" s="4"/>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="J47" s="4"/>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J49" s="4"/>
     </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="51" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J51" s="4"/>
     </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="53" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J53" s="4"/>
     </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="55" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J55" s="4"/>
     </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="57" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J57" s="4"/>
     </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="59" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J59" s="4"/>
     </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="61" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J61" s="4"/>
     </row>
-    <row r="63" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="63" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J63" s="4"/>
     </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J65" s="4"/>
     </row>
-    <row r="67" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="67" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J67" s="4"/>
     </row>
-    <row r="69" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="69" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J69" s="4"/>
     </row>
-    <row r="71" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="71" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J71" s="4"/>
     </row>
-    <row r="73" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="73" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J73" s="4"/>
     </row>
-    <row r="75" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="75" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J75" s="4"/>
     </row>
-    <row r="77" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="77" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J77" s="4"/>
     </row>
-    <row r="79" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="79" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J79" s="4"/>
     </row>
-    <row r="81" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="81" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J81" s="4"/>
     </row>
-    <row r="83" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="83" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J83" s="4"/>
     </row>
-    <row r="85" spans="10:10" x14ac:dyDescent="0.5">
+    <row r="85" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J85" s="4"/>
     </row>
   </sheetData>
@@ -15010,7 +15733,1788 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CFFFFC-40D2-4CE7-82A6-7ADBA94BBBBB}">
+  <dimension ref="A1:M102"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>522</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>523</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>524</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>525</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B2" t="s">
+        <v>528</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>530</v>
+      </c>
+      <c r="B3" t="s">
+        <v>531</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>532</v>
+      </c>
+      <c r="E3" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>530</v>
+      </c>
+      <c r="B4" t="s">
+        <v>531</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>534</v>
+      </c>
+      <c r="B5" t="s">
+        <v>535</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>536</v>
+      </c>
+      <c r="E5" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>534</v>
+      </c>
+      <c r="B6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>538</v>
+      </c>
+      <c r="E6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>534</v>
+      </c>
+      <c r="B7" t="s">
+        <v>535</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>540</v>
+      </c>
+      <c r="E7" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>542</v>
+      </c>
+      <c r="B8" t="s">
+        <v>543</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>544</v>
+      </c>
+      <c r="E8" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>542</v>
+      </c>
+      <c r="B9" t="s">
+        <v>543</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>542</v>
+      </c>
+      <c r="B10" t="s">
+        <v>543</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>547</v>
+      </c>
+      <c r="E10" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>549</v>
+      </c>
+      <c r="B11" t="s">
+        <v>550</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>551</v>
+      </c>
+      <c r="E11" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>549</v>
+      </c>
+      <c r="B12" t="s">
+        <v>550</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>553</v>
+      </c>
+      <c r="E12" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>555</v>
+      </c>
+      <c r="B13" t="s">
+        <v>556</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" t="s">
+        <v>557</v>
+      </c>
+      <c r="E13" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>555</v>
+      </c>
+      <c r="B14" t="s">
+        <v>556</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>559</v>
+      </c>
+      <c r="E14" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>555</v>
+      </c>
+      <c r="B15" t="s">
+        <v>556</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>561</v>
+      </c>
+      <c r="E15" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>563</v>
+      </c>
+      <c r="B16" t="s">
+        <v>564</v>
+      </c>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>538</v>
+      </c>
+      <c r="E16" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>563</v>
+      </c>
+      <c r="B17" t="s">
+        <v>564</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>536</v>
+      </c>
+      <c r="E17" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>563</v>
+      </c>
+      <c r="B18" t="s">
+        <v>564</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
+        <v>565</v>
+      </c>
+      <c r="E18" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>574</v>
+      </c>
+      <c r="B22" t="s">
+        <v>575</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>576</v>
+      </c>
+      <c r="E22" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>574</v>
+      </c>
+      <c r="B23" t="s">
+        <v>575</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>578</v>
+      </c>
+      <c r="E23" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>574</v>
+      </c>
+      <c r="B24" t="s">
+        <v>575</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>580</v>
+      </c>
+      <c r="E24" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>574</v>
+      </c>
+      <c r="B25" t="s">
+        <v>575</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>582</v>
+      </c>
+      <c r="E25" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>574</v>
+      </c>
+      <c r="B26" t="s">
+        <v>575</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>584</v>
+      </c>
+      <c r="E26" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>586</v>
+      </c>
+      <c r="B27" t="s">
+        <v>587</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" t="s">
+        <v>588</v>
+      </c>
+      <c r="E27" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>586</v>
+      </c>
+      <c r="B28" t="s">
+        <v>587</v>
+      </c>
+      <c r="C28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" t="s">
+        <v>590</v>
+      </c>
+      <c r="E28" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>592</v>
+      </c>
+      <c r="B29" t="s">
+        <v>593</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>594</v>
+      </c>
+      <c r="E29" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>592</v>
+      </c>
+      <c r="B30" t="s">
+        <v>593</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" t="s">
+        <v>596</v>
+      </c>
+      <c r="E30" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>592</v>
+      </c>
+      <c r="B31" t="s">
+        <v>593</v>
+      </c>
+      <c r="C31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" t="s">
+        <v>598</v>
+      </c>
+      <c r="E31" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>592</v>
+      </c>
+      <c r="B32" t="s">
+        <v>593</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>600</v>
+      </c>
+      <c r="E32" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>592</v>
+      </c>
+      <c r="B33" t="s">
+        <v>593</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>602</v>
+      </c>
+      <c r="E33" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>604</v>
+      </c>
+      <c r="B34" t="s">
+        <v>605</v>
+      </c>
+      <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" t="s">
+        <v>606</v>
+      </c>
+      <c r="E34" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>604</v>
+      </c>
+      <c r="B35" t="s">
+        <v>605</v>
+      </c>
+      <c r="C35" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" t="s">
+        <v>608</v>
+      </c>
+      <c r="E35" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>604</v>
+      </c>
+      <c r="B36" t="s">
+        <v>605</v>
+      </c>
+      <c r="C36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" t="s">
+        <v>610</v>
+      </c>
+      <c r="E36" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>604</v>
+      </c>
+      <c r="B37" t="s">
+        <v>605</v>
+      </c>
+      <c r="C37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" t="s">
+        <v>612</v>
+      </c>
+      <c r="E37" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>604</v>
+      </c>
+      <c r="B38" t="s">
+        <v>605</v>
+      </c>
+      <c r="C38" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" t="s">
+        <v>614</v>
+      </c>
+      <c r="E38" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>616</v>
+      </c>
+      <c r="B39" t="s">
+        <v>617</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+      <c r="D39" s="43" t="s">
+        <v>618</v>
+      </c>
+      <c r="E39" s="43" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>616</v>
+      </c>
+      <c r="B40" t="s">
+        <v>617</v>
+      </c>
+      <c r="C40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="43" t="s">
+        <v>620</v>
+      </c>
+      <c r="E40" s="43" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>616</v>
+      </c>
+      <c r="B41" t="s">
+        <v>617</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+      <c r="D41" s="43" t="s">
+        <v>622</v>
+      </c>
+      <c r="E41" s="43" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>616</v>
+      </c>
+      <c r="B42" t="s">
+        <v>617</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" s="43" t="s">
+        <v>624</v>
+      </c>
+      <c r="E42" s="43" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>616</v>
+      </c>
+      <c r="B43" t="s">
+        <v>617</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="43" t="s">
+        <v>626</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>616</v>
+      </c>
+      <c r="B44" t="s">
+        <v>617</v>
+      </c>
+      <c r="C44" t="s">
+        <v>26</v>
+      </c>
+      <c r="D44" s="43" t="s">
+        <v>628</v>
+      </c>
+      <c r="E44" s="43" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>616</v>
+      </c>
+      <c r="B45" t="s">
+        <v>617</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="43" t="s">
+        <v>630</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>616</v>
+      </c>
+      <c r="B46" t="s">
+        <v>617</v>
+      </c>
+      <c r="C46" t="s">
+        <v>26</v>
+      </c>
+      <c r="D46" s="43" t="s">
+        <v>632</v>
+      </c>
+      <c r="E46" s="43" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>616</v>
+      </c>
+      <c r="B47" t="s">
+        <v>617</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>634</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>616</v>
+      </c>
+      <c r="B48" t="s">
+        <v>617</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>636</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>637</v>
+      </c>
+      <c r="M48" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>616</v>
+      </c>
+      <c r="B49" t="s">
+        <v>617</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="43" t="s">
+        <v>639</v>
+      </c>
+      <c r="E49" s="43" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>641</v>
+      </c>
+      <c r="B50" t="s">
+        <v>642</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
+        <v>643</v>
+      </c>
+      <c r="E50" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>641</v>
+      </c>
+      <c r="B51" t="s">
+        <v>642</v>
+      </c>
+      <c r="C51" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="44" t="s">
+        <v>645</v>
+      </c>
+      <c r="E51" s="43" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>641</v>
+      </c>
+      <c r="B52" t="s">
+        <v>642</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D52" s="44" t="s">
+        <v>647</v>
+      </c>
+      <c r="E52" s="43" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>641</v>
+      </c>
+      <c r="B53" t="s">
+        <v>642</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53" s="43" t="s">
+        <v>649</v>
+      </c>
+      <c r="E53" s="43" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>641</v>
+      </c>
+      <c r="B54" t="s">
+        <v>642</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" s="43" t="s">
+        <v>651</v>
+      </c>
+      <c r="E54" s="43" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>641</v>
+      </c>
+      <c r="B55" t="s">
+        <v>642</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55" s="43" t="s">
+        <v>653</v>
+      </c>
+      <c r="E55" s="43" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>641</v>
+      </c>
+      <c r="B56" t="s">
+        <v>642</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56" s="43" t="s">
+        <v>655</v>
+      </c>
+      <c r="E56" s="43" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>641</v>
+      </c>
+      <c r="B57" t="s">
+        <v>642</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="43" t="s">
+        <v>643</v>
+      </c>
+      <c r="E57" s="43" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>641</v>
+      </c>
+      <c r="B58" t="s">
+        <v>642</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" s="43" t="s">
+        <v>657</v>
+      </c>
+      <c r="E58" s="43" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>641</v>
+      </c>
+      <c r="B59" t="s">
+        <v>642</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59" s="43" t="s">
+        <v>659</v>
+      </c>
+      <c r="E59" s="43" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>641</v>
+      </c>
+      <c r="B60" t="s">
+        <v>642</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="43" t="s">
+        <v>645</v>
+      </c>
+      <c r="E60" s="43" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>641</v>
+      </c>
+      <c r="B61" t="s">
+        <v>642</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61" s="43" t="s">
+        <v>661</v>
+      </c>
+      <c r="E61" s="43" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>641</v>
+      </c>
+      <c r="B62" t="s">
+        <v>642</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" s="43" t="s">
+        <v>663</v>
+      </c>
+      <c r="E62" s="43" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>641</v>
+      </c>
+      <c r="B63" t="s">
+        <v>642</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="43" t="s">
+        <v>665</v>
+      </c>
+      <c r="E63" s="43" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>641</v>
+      </c>
+      <c r="B64" t="s">
+        <v>642</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64" s="43" t="s">
+        <v>667</v>
+      </c>
+      <c r="E64" s="43" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>641</v>
+      </c>
+      <c r="B65" t="s">
+        <v>642</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" s="43" t="s">
+        <v>669</v>
+      </c>
+      <c r="E65" s="43" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>641</v>
+      </c>
+      <c r="B66" t="s">
+        <v>642</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66" s="43" t="s">
+        <v>647</v>
+      </c>
+      <c r="E66" s="43" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>671</v>
+      </c>
+      <c r="B67" t="s">
+        <v>672</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67" s="43" t="s">
+        <v>673</v>
+      </c>
+      <c r="E67" s="43" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>671</v>
+      </c>
+      <c r="B68" t="s">
+        <v>672</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68" s="43" t="s">
+        <v>675</v>
+      </c>
+      <c r="E68" s="43" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>671</v>
+      </c>
+      <c r="B69" t="s">
+        <v>672</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" s="43" t="s">
+        <v>677</v>
+      </c>
+      <c r="E69" s="43" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>671</v>
+      </c>
+      <c r="B70" t="s">
+        <v>672</v>
+      </c>
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70" s="43" t="s">
+        <v>679</v>
+      </c>
+      <c r="E70" s="43" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>671</v>
+      </c>
+      <c r="B71" t="s">
+        <v>672</v>
+      </c>
+      <c r="C71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71" s="43" t="s">
+        <v>681</v>
+      </c>
+      <c r="E71" s="43" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>671</v>
+      </c>
+      <c r="B72" t="s">
+        <v>672</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72" s="43" t="s">
+        <v>547</v>
+      </c>
+      <c r="E72" s="43" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>671</v>
+      </c>
+      <c r="B73" t="s">
+        <v>672</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73" s="43" t="s">
+        <v>683</v>
+      </c>
+      <c r="E73" s="43" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>671</v>
+      </c>
+      <c r="B74" t="s">
+        <v>672</v>
+      </c>
+      <c r="C74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74" s="43" t="s">
+        <v>685</v>
+      </c>
+      <c r="E74" s="43" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>671</v>
+      </c>
+      <c r="B75" t="s">
+        <v>672</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75" s="43" t="s">
+        <v>544</v>
+      </c>
+      <c r="E75" s="43" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>671</v>
+      </c>
+      <c r="B76" t="s">
+        <v>672</v>
+      </c>
+      <c r="C76" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="43" t="s">
+        <v>75</v>
+      </c>
+      <c r="E76" s="43" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>671</v>
+      </c>
+      <c r="B77" t="s">
+        <v>672</v>
+      </c>
+      <c r="C77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77" s="43" t="s">
+        <v>687</v>
+      </c>
+      <c r="E77" s="43" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>671</v>
+      </c>
+      <c r="B78" t="s">
+        <v>672</v>
+      </c>
+      <c r="C78" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" s="43" t="s">
+        <v>689</v>
+      </c>
+      <c r="E78" s="43" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>671</v>
+      </c>
+      <c r="B79" t="s">
+        <v>672</v>
+      </c>
+      <c r="C79" t="s">
+        <v>26</v>
+      </c>
+      <c r="D79" s="43" t="s">
+        <v>691</v>
+      </c>
+      <c r="E79" s="43" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>671</v>
+      </c>
+      <c r="B80" t="s">
+        <v>672</v>
+      </c>
+      <c r="C80" t="s">
+        <v>26</v>
+      </c>
+      <c r="D80" s="43" t="s">
+        <v>693</v>
+      </c>
+      <c r="E80" s="43" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>671</v>
+      </c>
+      <c r="B81" t="s">
+        <v>672</v>
+      </c>
+      <c r="C81" t="s">
+        <v>26</v>
+      </c>
+      <c r="D81" s="43" t="s">
+        <v>695</v>
+      </c>
+      <c r="E81" s="43" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>697</v>
+      </c>
+      <c r="B82" t="s">
+        <v>698</v>
+      </c>
+      <c r="C82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82" s="43" t="s">
+        <v>699</v>
+      </c>
+      <c r="E82" s="43" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>697</v>
+      </c>
+      <c r="B83" t="s">
+        <v>698</v>
+      </c>
+      <c r="C83" t="s">
+        <v>26</v>
+      </c>
+      <c r="D83" s="43" t="s">
+        <v>701</v>
+      </c>
+      <c r="E83" s="43" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>697</v>
+      </c>
+      <c r="B84" t="s">
+        <v>698</v>
+      </c>
+      <c r="C84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" s="43" t="s">
+        <v>703</v>
+      </c>
+      <c r="E84" s="43" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>697</v>
+      </c>
+      <c r="B85" t="s">
+        <v>698</v>
+      </c>
+      <c r="C85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" s="43" t="s">
+        <v>705</v>
+      </c>
+      <c r="E85" s="43" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>697</v>
+      </c>
+      <c r="B86" t="s">
+        <v>698</v>
+      </c>
+      <c r="C86" t="s">
+        <v>26</v>
+      </c>
+      <c r="D86" s="43" t="s">
+        <v>707</v>
+      </c>
+      <c r="E86" s="43" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>697</v>
+      </c>
+      <c r="B87" t="s">
+        <v>698</v>
+      </c>
+      <c r="C87" t="s">
+        <v>26</v>
+      </c>
+      <c r="D87" s="43" t="s">
+        <v>709</v>
+      </c>
+      <c r="E87" s="43" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>697</v>
+      </c>
+      <c r="B88" t="s">
+        <v>698</v>
+      </c>
+      <c r="C88" t="s">
+        <v>26</v>
+      </c>
+      <c r="D88" s="43" t="s">
+        <v>711</v>
+      </c>
+      <c r="E88" s="43" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>697</v>
+      </c>
+      <c r="B89" t="s">
+        <v>698</v>
+      </c>
+      <c r="C89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D89" s="43" t="s">
+        <v>713</v>
+      </c>
+      <c r="E89" s="43" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>715</v>
+      </c>
+      <c r="B90" t="s">
+        <v>716</v>
+      </c>
+      <c r="C90" t="s">
+        <v>26</v>
+      </c>
+      <c r="D90" t="s">
+        <v>717</v>
+      </c>
+      <c r="E90" s="45" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>715</v>
+      </c>
+      <c r="B91" t="s">
+        <v>716</v>
+      </c>
+      <c r="C91" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" t="s">
+        <v>719</v>
+      </c>
+      <c r="E91" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>721</v>
+      </c>
+      <c r="B92" t="s">
+        <v>722</v>
+      </c>
+      <c r="C92" t="s">
+        <v>723</v>
+      </c>
+      <c r="D92" s="44" t="s">
+        <v>724</v>
+      </c>
+      <c r="E92" s="44" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>721</v>
+      </c>
+      <c r="B93" t="s">
+        <v>722</v>
+      </c>
+      <c r="C93" t="s">
+        <v>723</v>
+      </c>
+      <c r="D93" s="44" t="s">
+        <v>726</v>
+      </c>
+      <c r="E93" s="44" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>721</v>
+      </c>
+      <c r="B94" t="s">
+        <v>722</v>
+      </c>
+      <c r="C94" t="s">
+        <v>723</v>
+      </c>
+      <c r="D94" s="44" t="s">
+        <v>728</v>
+      </c>
+      <c r="E94" s="44" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>721</v>
+      </c>
+      <c r="B95" t="s">
+        <v>722</v>
+      </c>
+      <c r="C95" t="s">
+        <v>723</v>
+      </c>
+      <c r="D95" s="44" t="s">
+        <v>730</v>
+      </c>
+      <c r="E95" s="44" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>721</v>
+      </c>
+      <c r="B96" t="s">
+        <v>722</v>
+      </c>
+      <c r="C96" t="s">
+        <v>723</v>
+      </c>
+      <c r="D96" s="44" t="s">
+        <v>732</v>
+      </c>
+      <c r="E96" s="44" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>721</v>
+      </c>
+      <c r="B97" t="s">
+        <v>722</v>
+      </c>
+      <c r="C97" t="s">
+        <v>723</v>
+      </c>
+      <c r="D97" s="44" t="s">
+        <v>734</v>
+      </c>
+      <c r="E97" s="44" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>721</v>
+      </c>
+      <c r="B98" t="s">
+        <v>722</v>
+      </c>
+      <c r="C98" t="s">
+        <v>723</v>
+      </c>
+      <c r="D98" s="44" t="s">
+        <v>736</v>
+      </c>
+      <c r="E98" s="44" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>738</v>
+      </c>
+      <c r="B99" t="s">
+        <v>739</v>
+      </c>
+      <c r="C99" t="s">
+        <v>740</v>
+      </c>
+      <c r="D99" s="44" t="s">
+        <v>741</v>
+      </c>
+      <c r="E99" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>738</v>
+      </c>
+      <c r="B100" t="s">
+        <v>739</v>
+      </c>
+      <c r="C100" t="s">
+        <v>740</v>
+      </c>
+      <c r="D100" s="44" t="s">
+        <v>743</v>
+      </c>
+      <c r="E100" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>738</v>
+      </c>
+      <c r="B101" t="s">
+        <v>739</v>
+      </c>
+      <c r="C101" t="s">
+        <v>740</v>
+      </c>
+      <c r="D101" s="44" t="s">
+        <v>745</v>
+      </c>
+      <c r="E101" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>738</v>
+      </c>
+      <c r="B102" t="s">
+        <v>739</v>
+      </c>
+      <c r="C102" t="s">
+        <v>740</v>
+      </c>
+      <c r="D102" s="44" t="s">
+        <v>747</v>
+      </c>
+      <c r="E102" t="s">
+        <v>748</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Description0 xmlns="3dc215b4-4765-4137-95ef-e24fb8216673">Data and Metadata documentation will explain structure and content any QC manipulations that have been done to the data.</Description0>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EA3DD6FD0640724CAC6A104AA4040E53" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="95a591a9c1d64a7009b5597c446bd65f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3dc215b4-4765-4137-95ef-e24fb8216673" xmlns:ns3="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="63634f6e381b5ed55a864cdabf38da8d" ns2:_="" ns3:_="">
     <xsd:import namespace="3dc215b4-4765-4137-95ef-e24fb8216673"/>
@@ -15235,24 +17739,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C7FF019-6E9E-4327-8A98-09E2F73626E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3dc215b4-4765-4137-95ef-e24fb8216673"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Description0 xmlns="3dc215b4-4765-4137-95ef-e24fb8216673">Data and Metadata documentation will explain structure and content any QC manipulations that have been done to the data.</Description0>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9663087D-43C0-4E56-A8DA-483B09F130B4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69987298-F94B-4FAE-824D-77320F34A719}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15269,29 +17781,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9663087D-43C0-4E56-A8DA-483B09F130B4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C7FF019-6E9E-4327-8A98-09E2F73626E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3dc215b4-4765-4137-95ef-e24fb8216673"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="2634c873-c79e-4fdd-b8bf-a33e5fa5c27f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>